<commit_message>
For mercycorps/TolaActivity#2539, update colors, dynamically size instruction merged cells.
</commit_message>
<xml_diff>
--- a/indicators/bulk_import_files/BulkImportTemplate.xlsx
+++ b/indicators/bulk_import_files/BulkImportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjogdeo/Sites/tolaActivity/TolaActivity/indicators/bulk_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ECB236-1945-7F49-9EDE-F5C05D1357EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A38975-6C16-C146-97D2-6555E679A20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -891,15 +891,17 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1123,7 +1125,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1139,7 +1141,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5"/>
@@ -1179,7 +1181,7 @@
     </row>
     <row r="2" spans="1:36" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="38" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="10"/>
@@ -1219,7 +1221,7 @@
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="10"/>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
@@ -1257,13 +1259,13 @@
     </row>
     <row r="4" spans="1:36" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11"/>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="12"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
@@ -1297,7 +1299,7 @@
     </row>
     <row r="5" spans="1:36" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="38" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="10"/>
@@ -7457,10 +7459,7 @@
     <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <mergeCells count="1">
-    <mergeCell ref="B4:F4"/>
-  </mergeCells>
+  <sheetProtection insertRows="0" deleteColumns="0" deleteRows="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
For mercycorps/TolaActivity#2539, add help text to header cells and refine column width.
</commit_message>
<xml_diff>
--- a/indicators/bulk_import_files/BulkImportTemplate.xlsx
+++ b/indicators/bulk_import_files/BulkImportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjogdeo/Sites/tolaActivity/TolaActivity/indicators/bulk_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A38975-6C16-C146-97D2-6555E679A20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B0EE21-E4C6-0C45-B4FE-0057A5184288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,355 +26,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdoU
-    (2021-04-19 21:25:17)
-Provide an indicator statement of the precise information needed to assess whether intended changes have occurred.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdpM
-    (2021-04-19 21:25:17)
-Classifying indicators by sector allows us to filter and analyze related sets of indicators.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">======
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">ID#AAAAMDoJdoI
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">    (2021-04-19 21:25:17)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Identify the source of this indicator (e.g. Mercy Corps DIG, EC, USAID, etc.) If the indicator is brand new and created specifically for the program, enter "Custom"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdo4
-    (2021-04-19 21:25:17)
-Provide a long-form definition of the indicator and all key terms that need further detail for precise and reliable measurement. Anyone reading the definition should understand exactly what the indicator is measuring without any ambiguity.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdoc
-    (2021-04-19 21:25:17)
-Explain why the indicator was chosen for this program.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdo0
-    (2021-04-19 21:25:17)
-Enter a meaningful description of what the indicator uses as its standard unit (e.g. households, kilograms, kits, participants, etc.)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdok
-    (2021-04-19 21:25:17)
-This selection determines how results are calculated and displayed.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdoM
-    (2021-04-19 21:25:17)
-Provide an explanation for any target value/s assigned to this indicator. You might include calculations and any historical or secondary data sources used to estimate targets.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdpU
-    (2021-04-19 21:25:17)
-Enter a numeric value for the baseline. If a baseline is not yet known or not applicable, enter a zero or select the "Not applicable" checkbox. The baseline can always be updated at later point in time.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdoo
-    (2021-04-19 21:25:17)
-Is your program trying to achieve an increase (+) or decrease (-) in the indicator's unit of measure? This field is important for the accuracy of our "indicators on track" metric. For example, if we are tracking a decrease in cases of malnutrition, we will have exceeded our indicator target when the result is lower than the target.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdoE
-    (2021-04-19 21:25:17)
-This selection determines how the indicator's targets and results are organized and displayed. Target frequencies will vary depending on how frequently the program needs indicator data to properly manage and report on program progress.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdoQ
-    (2021-04-19 21:25:17)
-Identify the source of indicator data and the tools used to collect data (e.g., surveys, checklists, etc.) Indicate whether these tools already exist or will need to be developed.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdos
-    (2021-04-19 21:25:17)
-Explain the process used to collect data (e.g., population-based sampling with randomized selection, review of partner records, etc.) Explain how the means of verification or data sources will be collected. Describe the methodological approaches the indicator will apply for data collection.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdow
-    (2021-04-19 21:25:17)
-List all data points required for reporting. While some indicators require a single data point (# of students attending training), others require multiple data points for calculation. For example, to calculate the % of students graduated from a training course, the two data points would be # of students graduated (numerator) and # of students enrolled (denominator).</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdpE
-    (2021-04-19 21:25:17)
-List the people or team(s) responsible for data collection. This can include community volunteers, program team members, local partner(s), enumerators, consultants, etc.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdo8
-    (2021-04-19 21:25:17)
-The method of analysis should be detailed enough to allow an auditor or third party to reproduce the analysis or calculation and generate the same result.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdpA
-    (2021-04-19 21:25:17)
-Select the primary uses of the indicator and its intended audience. This is the most important field in an indicator plan, because it explains the utility of the indicator. If an indicator has no clear informational purpose, then it should not be tracked or measured. By articulating who needs the indicator data, why and what they need it for, teams ensure that only useful indicators are included in the program.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdog
-    (2021-04-19 21:25:17)
-Provide any additional details about how data quality will be ensured for this specific 
-indicator. Additional details may include specific roles and responsibilities of team members 
-for ensuring data quality and/or specific data sources to be verified, reviewed, or 
-triangulated, for example.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAMDoJdoA
-    (2021-04-19 21:25:17)
-List any limitations of the data used to calculate this indicator (e.g., issues with validity, reliability, accuracy, precision, and/or potential for double counting.) Data issues can be related to indicator design, data collection methods, and/or data analysis methods. Please be specific and explain how data issues were addressed.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-  <extLst>
-    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7micMo/NmS/b+/L8yHXH1WQHVzYYgQ=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -523,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -607,12 +258,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1117,15 +762,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFD8D8D8"/>
   </sheetPr>
   <dimension ref="A1:AJ933"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7462,7 +7107,6 @@
   <sheetProtection insertRows="0" deleteColumns="0" deleteRows="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
For mercycorps/TolaActivity#2539, modify indicator number behavior, adjust colors, shading, borders.
</commit_message>
<xml_diff>
--- a/indicators/bulk_import_files/BulkImportTemplate.xlsx
+++ b/indicators/bulk_import_files/BulkImportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjogdeo/Sites/tolaActivity/TolaActivity/indicators/bulk_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B0EE21-E4C6-0C45-B4FE-0057A5184288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D15502-8038-E64A-B748-FBFAE71415EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -768,9 +768,9 @@
   </sheetPr>
   <dimension ref="A1:AJ933"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
For mercycorps/TolaActivity#2539, add help text, tweak formatting.
</commit_message>
<xml_diff>
--- a/indicators/bulk_import_files/BulkImportTemplate.xlsx
+++ b/indicators/bulk_import_files/BulkImportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjogdeo/Sites/tolaActivity/TolaActivity/indicators/bulk_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D15502-8038-E64A-B748-FBFAE71415EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69275A92-123F-B94B-9DCE-305A4A47CDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7104,7 +7104,7 @@
     <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <sheetProtection insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection formatColumns="0" formatRows="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>

<commit_message>
For mercycorps/TolaActivity#2539, fix sheet name.
</commit_message>
<xml_diff>
--- a/indicators/bulk_import_files/BulkImportTemplate.xlsx
+++ b/indicators/bulk_import_files/BulkImportTemplate.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjogdeo/Sites/tolaActivity/TolaActivity/indicators/bulk_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69275A92-123F-B94B-9DCE-305A4A47CDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AA5A86-1AB8-9241-9FF6-E9AF3DF8648D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Import indicators" sheetId="1" r:id="rId1"/>
     <sheet name="Hidden" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -770,7 +770,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
For mercycorps/TolaActivity#2544, change baseline tooltip text.
</commit_message>
<xml_diff>
--- a/indicators/bulk_import_files/BulkImportTemplate.xlsx
+++ b/indicators/bulk_import_files/BulkImportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjogdeo/Sites/tolaActivity/TolaActivity/indicators/bulk_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AA5A86-1AB8-9241-9FF6-E9AF3DF8648D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B85A5E4-3ED3-7345-BF39-DB39C19F0312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -769,8 +769,8 @@
   <dimension ref="A1:AJ933"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>